<commit_message>
go back to orig data
</commit_message>
<xml_diff>
--- a/_data/WePlayData/CleanedWPCIncomingParentReflection-July2019.xlsx
+++ b/_data/WePlayData/CleanedWPCIncomingParentReflection-July2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renarepenning/Desktop/School/weplaynoladata/_data/WePlayData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAD23BF-5BEC-204A-B0DE-04FADB6C31CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F82D089-D3C2-2D43-A5C0-E93275F614C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="20120" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="20120" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -1704,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>